<commit_message>
Versione 6.0 per libro
</commit_message>
<xml_diff>
--- a/Shiny/Dati/50volumi.xlsx
+++ b/Shiny/Dati/50volumi.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MODUNIVAR\Shiny\Dati\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B1113E-07A6-41B2-867E-9386369CD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,17 +24,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Volume (mL o g)</t>
+    <t>Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +72,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -112,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -144,9 +158,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,6 +210,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,269 +403,267 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>9.9660978998690837</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>9.9876565513659727</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>9.9840829857021447</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>9.9762499125609168</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>9.985478953658486</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>9.9845911631382762</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>9.9790652770571171</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>9.966347261488437</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9.9880948186728631</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9.9883172628870227</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9.9756648982838954</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9.9883709703681518</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9.98153272708808</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9.9828889874152367</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9.973997890901984</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>9.9791621491567923</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9.9786628211041091</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>9.9945338847283267</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>9.985033976099686</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>9.9797675170157447</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>9.98161006687954</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>9.9766584357530803</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>9.9849568655008909</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>9.9760833404252764</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>9.9815138059603044</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>9.9858255502659006</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>9.9718180394666263</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>9.9834067145457368</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>9.9841787818695877</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>9.9873038747864769</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>9.9742074748610605</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>9.9752335704215795</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>9.9849726352295249</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>9.9773061851556406</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>9.9815481975929572</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>9.9773565184114261</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>9.9807356522979092</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>9.9932558045657345</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>9.9897677723311347</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>9.9731393351794679</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>9.9837531456251156</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>9.9889932921178399</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>9.9892381844802287</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>9.9853341102607658</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>9.9789043265082285</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>9.9788009797157713</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>9.979934452039771</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>9.9746345117273734</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>9.9766907519188237</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>9.9747410353848238</v>
       </c>
@@ -626,24 +674,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>